<commit_message>
Updated timeline for sitemap and wireframes
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952AB21B-EA94-4B8F-86D5-3DFD4D4F9A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419096F3-DD8E-4434-A670-E5C625814C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="503" windowWidth="24196" windowHeight="13094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,6 +925,18 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -932,18 +944,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="142" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1557,117 +1557,117 @@
         <v>29</v>
       </c>
       <c r="B3" s="63"/>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="88">
+      <c r="D3" s="87"/>
+      <c r="E3" s="85">
         <v>43983</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="85"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="82">
         <f>I5</f>
         <v>43983</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="82">
         <f>P5</f>
         <v>43990</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="82">
         <f>W5</f>
         <v>43997</v>
       </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="84"/>
+      <c r="AD4" s="82">
         <f>AD5</f>
         <v>44004</v>
       </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+      <c r="AE4" s="83"/>
+      <c r="AF4" s="83"/>
+      <c r="AG4" s="83"/>
+      <c r="AH4" s="83"/>
+      <c r="AI4" s="83"/>
+      <c r="AJ4" s="84"/>
+      <c r="AK4" s="82">
         <f>AK5</f>
         <v>44011</v>
       </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+      <c r="AL4" s="83"/>
+      <c r="AM4" s="83"/>
+      <c r="AN4" s="83"/>
+      <c r="AO4" s="83"/>
+      <c r="AP4" s="83"/>
+      <c r="AQ4" s="84"/>
+      <c r="AR4" s="82">
         <f>AR5</f>
         <v>44018</v>
       </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+      <c r="AS4" s="83"/>
+      <c r="AT4" s="83"/>
+      <c r="AU4" s="83"/>
+      <c r="AV4" s="83"/>
+      <c r="AW4" s="83"/>
+      <c r="AX4" s="84"/>
+      <c r="AY4" s="82">
         <f>AY5</f>
         <v>44025</v>
       </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+      <c r="AZ4" s="83"/>
+      <c r="BA4" s="83"/>
+      <c r="BB4" s="83"/>
+      <c r="BC4" s="83"/>
+      <c r="BD4" s="83"/>
+      <c r="BE4" s="84"/>
+      <c r="BF4" s="82">
         <f>BF5</f>
         <v>44032</v>
       </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+      <c r="BG4" s="83"/>
+      <c r="BH4" s="83"/>
+      <c r="BI4" s="83"/>
+      <c r="BJ4" s="83"/>
+      <c r="BK4" s="83"/>
+      <c r="BL4" s="84"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43983</v>
@@ -2381,13 +2381,13 @@
         <v>43985</v>
       </c>
       <c r="F10" s="64">
-        <f>E10+12</f>
-        <v>43997</v>
+        <f>E10+14</f>
+        <v>43999</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
@@ -2461,13 +2461,13 @@
         <v>43985</v>
       </c>
       <c r="F11" s="64">
-        <f>E11+12</f>
-        <v>43997</v>
+        <f>E11+14</f>
+        <v>43999</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
@@ -4262,6 +4262,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4269,11 +4274,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="D7:D21 D27 D33">

</xml_diff>

<commit_message>
Completed sitemap & wireframes
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419096F3-DD8E-4434-A670-E5C625814C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611A3054-3970-41A8-A590-C59A666B531A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="503" windowWidth="24196" windowHeight="13094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,6 +925,13 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -937,13 +944,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1512,9 +1512,9 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="142" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="73" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1557,117 +1557,117 @@
         <v>29</v>
       </c>
       <c r="B3" s="63"/>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="85">
+      <c r="D3" s="83"/>
+      <c r="E3" s="88">
         <v>43983</v>
       </c>
-      <c r="F3" s="85"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="85">
         <f>I5</f>
         <v>43983</v>
       </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="82">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f>P5</f>
         <v>43990</v>
       </c>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="82">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f>W5</f>
         <v>43997</v>
       </c>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
-      <c r="AB4" s="83"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="82">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f>AD5</f>
         <v>44004</v>
       </c>
-      <c r="AE4" s="83"/>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="83"/>
-      <c r="AH4" s="83"/>
-      <c r="AI4" s="83"/>
-      <c r="AJ4" s="84"/>
-      <c r="AK4" s="82">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f>AK5</f>
         <v>44011</v>
       </c>
-      <c r="AL4" s="83"/>
-      <c r="AM4" s="83"/>
-      <c r="AN4" s="83"/>
-      <c r="AO4" s="83"/>
-      <c r="AP4" s="83"/>
-      <c r="AQ4" s="84"/>
-      <c r="AR4" s="82">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f>AR5</f>
         <v>44018</v>
       </c>
-      <c r="AS4" s="83"/>
-      <c r="AT4" s="83"/>
-      <c r="AU4" s="83"/>
-      <c r="AV4" s="83"/>
-      <c r="AW4" s="83"/>
-      <c r="AX4" s="84"/>
-      <c r="AY4" s="82">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f>AY5</f>
         <v>44025</v>
       </c>
-      <c r="AZ4" s="83"/>
-      <c r="BA4" s="83"/>
-      <c r="BB4" s="83"/>
-      <c r="BC4" s="83"/>
-      <c r="BD4" s="83"/>
-      <c r="BE4" s="84"/>
-      <c r="BF4" s="82">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f>BF5</f>
         <v>44032</v>
       </c>
-      <c r="BG4" s="83"/>
-      <c r="BH4" s="83"/>
-      <c r="BI4" s="83"/>
-      <c r="BJ4" s="83"/>
-      <c r="BK4" s="83"/>
-      <c r="BL4" s="84"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43983</v>
@@ -2375,7 +2375,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="21">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="64">
         <v>43985</v>
@@ -2455,7 +2455,7 @@
         <v>45</v>
       </c>
       <c r="D11" s="21">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E11" s="64">
         <v>43985</v>
@@ -2535,7 +2535,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="21">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="64">
         <v>43990</v>
@@ -4262,11 +4262,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4274,6 +4269,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="D7:D21 D27 D33">

</xml_diff>